<commit_message>
Transport frozen pane settings
</commit_message>
<xml_diff>
--- a/playground/spreadsheet/DPL/Host/App_Data/Sample.xlsx
+++ b/playground/spreadsheet/DPL/Host/App_Data/Sample.xlsx
@@ -382,7 +382,10 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>